<commit_message>
Final Submit - Added comments
</commit_message>
<xml_diff>
--- a/src/test/resources/exceldata.xlsx
+++ b/src/test/resources/exceldata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prajchaudhary\IdeaProjects\HU_API_Main_Assignment\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{64A6CFD7-20D3-4CDF-93FC-FD7CCFA54422}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C2524B6-6514-48B0-8E7E-D61A685A2885}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4BD89A22-9B97-4890-9FBD-3114B2BD0B17}"/>
+    <workbookView xWindow="2120" yWindow="2120" windowWidth="14400" windowHeight="7360" xr2:uid="{4BD89A22-9B97-4890-9FBD-3114B2BD0B17}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
   <si>
     <t>name</t>
   </si>
@@ -88,6 +88,12 @@
   </si>
   <si>
     <t>mnvjhvh@visky.trim</t>
+  </si>
+  <si>
+    <t>krat</t>
+  </si>
+  <si>
+    <t>krat011@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -450,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B86EA6DF-0B72-44AA-A299-9568BF5561C0}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -548,6 +554,20 @@
         <v>13</v>
       </c>
     </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{D45895F5-A45C-4B7D-B239-E732D198C90E}"/>
@@ -555,8 +575,9 @@
     <hyperlink ref="C4" r:id="rId3" xr:uid="{8CB61085-9550-4422-8DFD-9EE43D302DBC}"/>
     <hyperlink ref="C5" r:id="rId4" xr:uid="{CC80E3E3-1042-455B-BC69-C238CE9756B1}"/>
     <hyperlink ref="C6" r:id="rId5" xr:uid="{B6F05361-806C-4436-9906-FA032173D045}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{D8FA65BD-9B4E-42F6-8371-A93D8413F934}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>